<commit_message>
added listbox and scrollbar
</commit_message>
<xml_diff>
--- a/try_controls_1/document/Layout_design.xlsx
+++ b/try_controls_1/document/Layout_design.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ASDProjects\PythonProjects\ASD_WinForms\try_controls_1\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B6C3BF-D4F5-4E6E-8361-DCD1E656EA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A72338-EBA8-47A9-9ED2-9FA99C3DD0D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28605" yWindow="1635" windowWidth="23460" windowHeight="14100" xr2:uid="{565E76EB-86A7-4188-BE72-7ACE8362D8A7}"/>
+    <workbookView xWindow="29280" yWindow="1470" windowWidth="23460" windowHeight="14100" xr2:uid="{565E76EB-86A7-4188-BE72-7ACE8362D8A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calculate" sheetId="5" r:id="rId1"/>
-    <sheet name="RockPaperScissors（1）" sheetId="1" r:id="rId2"/>
-    <sheet name="RockPaperScissors（2）" sheetId="2" r:id="rId3"/>
-    <sheet name="Login" sheetId="4" r:id="rId4"/>
-    <sheet name="SectionPaper" sheetId="3" r:id="rId5"/>
-    <sheet name="省市区县" sheetId="6" r:id="rId6"/>
+    <sheet name="CharactersAndPlayers" sheetId="7" r:id="rId1"/>
+    <sheet name="Calculate" sheetId="5" r:id="rId2"/>
+    <sheet name="RockPaperScissors（1）" sheetId="1" r:id="rId3"/>
+    <sheet name="RockPaperScissors（2）" sheetId="2" r:id="rId4"/>
+    <sheet name="Login" sheetId="4" r:id="rId5"/>
+    <sheet name="SectionPaper" sheetId="3" r:id="rId6"/>
+    <sheet name="省市区县" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>请输入挑战者昵称</t>
   </si>
@@ -150,7 +151,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -172,37 +173,274 @@
       </rPr>
       <t>2</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>结果是</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>▼</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>浙江省</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>杭州市</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>地址</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电视剧角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>演员名字1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>演员名字2</t>
+  </si>
+  <si>
+    <t>演员名字3</t>
+  </si>
+  <si>
+    <t>演员名字4</t>
+  </si>
+  <si>
+    <t>演员名字5</t>
+  </si>
+  <si>
+    <t>演员名字6</t>
+  </si>
+  <si>
+    <t>演员名字7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,339 +850,378 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1507,10 +1784,1529 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F7EE9D-4BDF-4F38-8EBD-C7A4C6C436DD}">
+  <dimension ref="B1:AQ32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.25" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.25" style="1"/>
+    <col min="2" max="33" width="4.25" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="4.25" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:33" s="38" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55">
+        <v>0</v>
+      </c>
+      <c r="D1" s="55">
+        <f>C1+20</f>
+        <v>20</v>
+      </c>
+      <c r="E1" s="55">
+        <f t="shared" ref="E1:AF1" si="0">D1+20</f>
+        <v>40</v>
+      </c>
+      <c r="F1" s="55">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G1" s="55">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H1" s="55">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I1" s="55">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="J1" s="55">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="K1" s="55">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="L1" s="55">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="M1" s="55">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="N1" s="55">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="O1" s="55">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="P1" s="55">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="Q1" s="55">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="R1" s="55">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="S1" s="55">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="T1" s="55">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+      <c r="U1" s="55">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="V1" s="55">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="W1" s="55">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="X1" s="55">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="Y1" s="55">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="Z1" s="55">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="AA1" s="55">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="AB1" s="55">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="AC1" s="55">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+      <c r="AD1" s="55">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+      <c r="AE1" s="55">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+      <c r="AF1" s="55">
+        <f t="shared" si="0"/>
+        <v>580</v>
+      </c>
+      <c r="AG1" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:33" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="39">
+        <v>0</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="39">
+        <f>B2+20</f>
+        <v>20</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="113" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="122" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
+      <c r="AC3" s="74"/>
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="74"/>
+      <c r="AF3" s="63"/>
+      <c r="AG3" s="29">
+        <f>AG2+20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="39">
+        <f t="shared" ref="B4:B31" si="1">B3+20</f>
+        <v>40</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="116" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="63"/>
+      <c r="AG4" s="29">
+        <f t="shared" ref="AG4:AG31" si="2">AG3+20</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="39">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="123" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74"/>
+      <c r="AF5" s="63"/>
+      <c r="AG5" s="29">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="39">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="116" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="123" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="118"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="74"/>
+      <c r="X6" s="74"/>
+      <c r="Y6" s="74"/>
+      <c r="Z6" s="74"/>
+      <c r="AA6" s="74"/>
+      <c r="AB6" s="74"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="74"/>
+      <c r="AF6" s="63"/>
+      <c r="AG6" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="39">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AF7" s="63"/>
+      <c r="AG7" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="39">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="123" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="63"/>
+      <c r="AG8" s="29">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="39">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="C9" s="59"/>
+      <c r="D9" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="120"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="124" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="X9" s="74"/>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+      <c r="AB9" s="74"/>
+      <c r="AC9" s="74"/>
+      <c r="AD9" s="74"/>
+      <c r="AE9" s="74"/>
+      <c r="AF9" s="63"/>
+      <c r="AG9" s="29">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="39">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="74"/>
+      <c r="AC10" s="74"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
+      <c r="AF10" s="63"/>
+      <c r="AG10" s="29">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="39">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
+      <c r="X11" s="74"/>
+      <c r="Y11" s="74"/>
+      <c r="Z11" s="74"/>
+      <c r="AA11" s="74"/>
+      <c r="AB11" s="74"/>
+      <c r="AC11" s="74"/>
+      <c r="AD11" s="74"/>
+      <c r="AE11" s="74"/>
+      <c r="AF11" s="63"/>
+      <c r="AG11" s="29">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="39">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="C12" s="59"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="74"/>
+      <c r="AC12" s="74"/>
+      <c r="AD12" s="74"/>
+      <c r="AE12" s="74"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="29">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="39">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+      <c r="X13" s="74"/>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="74"/>
+      <c r="AA13" s="74"/>
+      <c r="AB13" s="74"/>
+      <c r="AC13" s="74"/>
+      <c r="AD13" s="74"/>
+      <c r="AE13" s="74"/>
+      <c r="AF13" s="63"/>
+      <c r="AG13" s="29">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="39">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="74"/>
+      <c r="X14" s="74"/>
+      <c r="Y14" s="74"/>
+      <c r="Z14" s="74"/>
+      <c r="AA14" s="74"/>
+      <c r="AB14" s="74"/>
+      <c r="AC14" s="74"/>
+      <c r="AD14" s="74"/>
+      <c r="AE14" s="74"/>
+      <c r="AF14" s="63"/>
+      <c r="AG14" s="29">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="39">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="74"/>
+      <c r="Z15" s="74"/>
+      <c r="AA15" s="74"/>
+      <c r="AB15" s="74"/>
+      <c r="AC15" s="74"/>
+      <c r="AD15" s="74"/>
+      <c r="AE15" s="74"/>
+      <c r="AF15" s="63"/>
+      <c r="AG15" s="29">
+        <f t="shared" si="2"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="39">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
+      <c r="Z16" s="74"/>
+      <c r="AA16" s="74"/>
+      <c r="AB16" s="74"/>
+      <c r="AC16" s="74"/>
+      <c r="AD16" s="74"/>
+      <c r="AE16" s="74"/>
+      <c r="AF16" s="63"/>
+      <c r="AG16" s="29">
+        <f t="shared" si="2"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="39">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="C17" s="59"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="74"/>
+      <c r="X17" s="74"/>
+      <c r="Y17" s="74"/>
+      <c r="Z17" s="74"/>
+      <c r="AA17" s="74"/>
+      <c r="AB17" s="74"/>
+      <c r="AC17" s="74"/>
+      <c r="AD17" s="74"/>
+      <c r="AE17" s="74"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="29">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="39">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="74"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
+      <c r="S18" s="74"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="74"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="74"/>
+      <c r="X18" s="74"/>
+      <c r="Y18" s="74"/>
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="74"/>
+      <c r="AB18" s="74"/>
+      <c r="AC18" s="74"/>
+      <c r="AD18" s="74"/>
+      <c r="AE18" s="74"/>
+      <c r="AF18" s="63"/>
+      <c r="AG18" s="29">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="39">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="74"/>
+      <c r="Y19" s="74"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+      <c r="AB19" s="74"/>
+      <c r="AC19" s="74"/>
+      <c r="AD19" s="74"/>
+      <c r="AE19" s="74"/>
+      <c r="AF19" s="63"/>
+      <c r="AG19" s="29">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="39">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="C20" s="59"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="74"/>
+      <c r="S20" s="74"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="74"/>
+      <c r="Y20" s="74"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="74"/>
+      <c r="AB20" s="74"/>
+      <c r="AC20" s="74"/>
+      <c r="AD20" s="74"/>
+      <c r="AE20" s="74"/>
+      <c r="AF20" s="63"/>
+      <c r="AG20" s="29">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="39">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+      <c r="C21" s="59"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="74"/>
+      <c r="R21" s="74"/>
+      <c r="S21" s="74"/>
+      <c r="T21" s="74"/>
+      <c r="U21" s="74"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="74"/>
+      <c r="X21" s="74"/>
+      <c r="Y21" s="74"/>
+      <c r="Z21" s="74"/>
+      <c r="AA21" s="74"/>
+      <c r="AB21" s="74"/>
+      <c r="AC21" s="74"/>
+      <c r="AD21" s="74"/>
+      <c r="AE21" s="74"/>
+      <c r="AF21" s="63"/>
+      <c r="AG21" s="29">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="39">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="74"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="74"/>
+      <c r="X22" s="74"/>
+      <c r="Y22" s="74"/>
+      <c r="Z22" s="74"/>
+      <c r="AA22" s="74"/>
+      <c r="AB22" s="74"/>
+      <c r="AC22" s="74"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="74"/>
+      <c r="AF22" s="63"/>
+      <c r="AG22" s="29">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="39">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="74"/>
+      <c r="Z23" s="74"/>
+      <c r="AA23" s="74"/>
+      <c r="AB23" s="74"/>
+      <c r="AC23" s="74"/>
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="74"/>
+      <c r="AF23" s="63"/>
+      <c r="AG23" s="29">
+        <f t="shared" si="2"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="24" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="39">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="C24" s="59"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="74"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="74"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="74"/>
+      <c r="X24" s="74"/>
+      <c r="Y24" s="74"/>
+      <c r="Z24" s="74"/>
+      <c r="AA24" s="74"/>
+      <c r="AB24" s="74"/>
+      <c r="AC24" s="74"/>
+      <c r="AD24" s="74"/>
+      <c r="AE24" s="74"/>
+      <c r="AF24" s="63"/>
+      <c r="AG24" s="29">
+        <f t="shared" si="2"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="39">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="74"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="74"/>
+      <c r="AF25" s="63"/>
+      <c r="AG25" s="29">
+        <f t="shared" si="2"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="39">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="74"/>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="74"/>
+      <c r="S26" s="74"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="74"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="74"/>
+      <c r="X26" s="74"/>
+      <c r="Y26" s="74"/>
+      <c r="Z26" s="74"/>
+      <c r="AA26" s="74"/>
+      <c r="AB26" s="74"/>
+      <c r="AC26" s="74"/>
+      <c r="AD26" s="74"/>
+      <c r="AE26" s="74"/>
+      <c r="AF26" s="63"/>
+      <c r="AG26" s="29">
+        <f t="shared" si="2"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="39">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="74"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="74"/>
+      <c r="S27" s="74"/>
+      <c r="T27" s="74"/>
+      <c r="U27" s="74"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="74"/>
+      <c r="X27" s="74"/>
+      <c r="Y27" s="74"/>
+      <c r="Z27" s="74"/>
+      <c r="AA27" s="74"/>
+      <c r="AB27" s="74"/>
+      <c r="AC27" s="74"/>
+      <c r="AD27" s="74"/>
+      <c r="AE27" s="74"/>
+      <c r="AF27" s="63"/>
+      <c r="AG27" s="29">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="39">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="74"/>
+      <c r="S28" s="74"/>
+      <c r="T28" s="74"/>
+      <c r="U28" s="74"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="74"/>
+      <c r="X28" s="74"/>
+      <c r="Y28" s="74"/>
+      <c r="Z28" s="74"/>
+      <c r="AA28" s="74"/>
+      <c r="AB28" s="74"/>
+      <c r="AC28" s="74"/>
+      <c r="AD28" s="74"/>
+      <c r="AE28" s="74"/>
+      <c r="AF28" s="63"/>
+      <c r="AG28" s="29">
+        <f t="shared" si="2"/>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="29" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="39">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="74"/>
+      <c r="Z29" s="74"/>
+      <c r="AA29" s="74"/>
+      <c r="AB29" s="74"/>
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="74"/>
+      <c r="AE29" s="74"/>
+      <c r="AF29" s="63"/>
+      <c r="AG29" s="29">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="30" spans="2:43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="39">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+      <c r="C30" s="59"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="74"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="74"/>
+      <c r="S30" s="74"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="74"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="74"/>
+      <c r="X30" s="74"/>
+      <c r="Y30" s="74"/>
+      <c r="Z30" s="74"/>
+      <c r="AA30" s="74"/>
+      <c r="AB30" s="74"/>
+      <c r="AC30" s="74"/>
+      <c r="AD30" s="74"/>
+      <c r="AE30" s="74"/>
+      <c r="AF30" s="63"/>
+      <c r="AG30" s="29">
+        <f t="shared" si="2"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="31" spans="2:43" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="39">
+        <f t="shared" si="1"/>
+        <v>580</v>
+      </c>
+      <c r="C31" s="64"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="65"/>
+      <c r="T31" s="65"/>
+      <c r="U31" s="65"/>
+      <c r="V31" s="65"/>
+      <c r="W31" s="65"/>
+      <c r="X31" s="65"/>
+      <c r="Y31" s="65"/>
+      <c r="Z31" s="65"/>
+      <c r="AA31" s="65"/>
+      <c r="AB31" s="65"/>
+      <c r="AC31" s="65"/>
+      <c r="AD31" s="65"/>
+      <c r="AE31" s="65"/>
+      <c r="AF31" s="66"/>
+      <c r="AG31" s="29">
+        <f t="shared" si="2"/>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="32" spans="2:43" s="38" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="29">
+        <v>0</v>
+      </c>
+      <c r="D32" s="29">
+        <f>C32+20</f>
+        <v>20</v>
+      </c>
+      <c r="E32" s="29">
+        <f t="shared" ref="E32:AF32" si="3">D32+20</f>
+        <v>40</v>
+      </c>
+      <c r="F32" s="29">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="G32" s="29">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="H32" s="29">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="I32" s="29">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="J32" s="29">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="K32" s="29">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="L32" s="29">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="M32" s="29">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N32" s="29">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="O32" s="29">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="P32" s="29">
+        <f t="shared" si="3"/>
+        <v>260</v>
+      </c>
+      <c r="Q32" s="29">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="R32" s="29">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="S32" s="29">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+      <c r="T32" s="29">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="U32" s="29">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="V32" s="29">
+        <f t="shared" si="3"/>
+        <v>380</v>
+      </c>
+      <c r="W32" s="29">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="X32" s="29">
+        <f t="shared" si="3"/>
+        <v>420</v>
+      </c>
+      <c r="Y32" s="29">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+      <c r="Z32" s="29">
+        <f t="shared" si="3"/>
+        <v>460</v>
+      </c>
+      <c r="AA32" s="29">
+        <f t="shared" si="3"/>
+        <v>480</v>
+      </c>
+      <c r="AB32" s="29">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="AC32" s="29">
+        <f t="shared" si="3"/>
+        <v>520</v>
+      </c>
+      <c r="AD32" s="29">
+        <f t="shared" si="3"/>
+        <v>540</v>
+      </c>
+      <c r="AE32" s="29">
+        <f t="shared" si="3"/>
+        <v>560</v>
+      </c>
+      <c r="AF32" s="29">
+        <f t="shared" si="3"/>
+        <v>580</v>
+      </c>
+      <c r="AG32" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ32" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F635F75-E57B-4532-8B3F-308D742CE3A4}">
   <dimension ref="B1:AQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
@@ -1711,10 +3507,10 @@
       <c r="L3" s="61"/>
       <c r="M3" s="62"/>
       <c r="N3" s="33"/>
-      <c r="O3" s="74" t="s">
+      <c r="O3" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="75"/>
+      <c r="P3" s="77"/>
       <c r="Q3" s="33"/>
       <c r="R3" s="61"/>
       <c r="S3" s="62"/>
@@ -2988,13 +4784,13 @@
   <mergeCells count="1">
     <mergeCell ref="O3:P3"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87047569-6F4A-4D23-804C-95AEA7D52317}">
   <dimension ref="B1:AG32"/>
   <sheetViews>
@@ -3230,16 +5026,16 @@
       <c r="K4" s="8"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="89" t="s">
+      <c r="N4" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="93"/>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
       <c r="V4" s="9"/>
       <c r="W4" s="9"/>
       <c r="X4" s="9" t="s">
@@ -3274,23 +5070,23 @@
       <c r="K5" s="14"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="90"/>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="79"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="84"/>
+      <c r="Z5" s="84"/>
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="85"/>
       <c r="AE5" s="9"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="29">
@@ -3522,18 +5318,18 @@
       <c r="K11" s="14"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="91" t="s">
+      <c r="N11" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="O11" s="92"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="93"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="96"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="100" t="s">
+      <c r="T11" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="101"/>
+      <c r="U11" s="104"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="19"/>
@@ -3566,16 +5362,16 @@
       <c r="K12" s="14"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="94"/>
-      <c r="O12" s="95"/>
-      <c r="P12" s="95"/>
-      <c r="Q12" s="95"/>
-      <c r="R12" s="96"/>
+      <c r="N12" s="97"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="99"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="102">
+      <c r="T12" s="105">
         <v>5</v>
       </c>
-      <c r="U12" s="103"/>
+      <c r="U12" s="106"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="19"/>
@@ -3608,14 +5404,14 @@
       <c r="K13" s="24"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="98"/>
-      <c r="R13" s="99"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="102"/>
       <c r="S13" s="9"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="105"/>
+      <c r="T13" s="107"/>
+      <c r="U13" s="108"/>
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
       <c r="X13" s="25"/>
@@ -3679,25 +5475,25 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="81"/>
-      <c r="S15" s="81"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="82"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="87"/>
+      <c r="T15" s="87"/>
+      <c r="U15" s="88"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="17"/>
@@ -3720,23 +5516,23 @@
         <v>280</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="85"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="90"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="90"/>
+      <c r="U16" s="91"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="19"/>
@@ -3759,27 +5555,27 @@
         <v>300</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="E17" s="86" t="s">
+      <c r="E17" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="88"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="78"/>
+      <c r="N17" s="80"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="76" t="s">
+      <c r="P17" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="19"/>
@@ -3802,27 +5598,27 @@
         <v>320</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="E18" s="86" t="s">
+      <c r="E18" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="88"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="78"/>
+      <c r="N18" s="80"/>
       <c r="O18" s="9"/>
-      <c r="P18" s="76" t="s">
+      <c r="P18" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="76"/>
-      <c r="R18" s="76"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="76"/>
-      <c r="U18" s="76"/>
+      <c r="Q18" s="81"/>
+      <c r="R18" s="81"/>
+      <c r="S18" s="81"/>
+      <c r="T18" s="81"/>
+      <c r="U18" s="81"/>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="19"/>
@@ -3847,27 +5643,27 @@
         <v>340</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="E19" s="86" t="s">
+      <c r="E19" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="88"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="80"/>
       <c r="O19" s="9"/>
-      <c r="P19" s="76" t="s">
+      <c r="P19" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="76"/>
-      <c r="U19" s="76"/>
+      <c r="Q19" s="81"/>
+      <c r="R19" s="81"/>
+      <c r="S19" s="81"/>
+      <c r="T19" s="81"/>
+      <c r="U19" s="81"/>
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
       <c r="X19" s="19"/>
@@ -3890,27 +5686,27 @@
         <v>360</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="E20" s="86" t="s">
+      <c r="E20" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="87"/>
-      <c r="K20" s="87"/>
-      <c r="L20" s="87"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="88"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="80"/>
       <c r="O20" s="9"/>
-      <c r="P20" s="76" t="s">
+      <c r="P20" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
-      <c r="T20" s="76"/>
-      <c r="U20" s="76"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="81"/>
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81"/>
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
       <c r="X20" s="19"/>
@@ -3933,27 +5729,27 @@
         <v>380</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="E21" s="86" t="s">
+      <c r="E21" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="88"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="78"/>
+      <c r="N21" s="80"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="76" t="s">
+      <c r="P21" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q21" s="76"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="76"/>
-      <c r="T21" s="76"/>
-      <c r="U21" s="76"/>
+      <c r="Q21" s="81"/>
+      <c r="R21" s="81"/>
+      <c r="S21" s="81"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="81"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="25"/>
@@ -3976,27 +5772,27 @@
         <v>400</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="E22" s="86" t="s">
+      <c r="E22" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="88"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="80"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="76" t="s">
+      <c r="P22" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q22" s="76"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="76"/>
-      <c r="T22" s="76"/>
-      <c r="U22" s="76"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="81"/>
+      <c r="S22" s="81"/>
+      <c r="T22" s="81"/>
+      <c r="U22" s="81"/>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="AE22" s="9"/>
@@ -4012,27 +5808,27 @@
         <v>420</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="E23" s="86" t="s">
+      <c r="E23" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="88"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="80"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="76" t="s">
+      <c r="P23" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="76"/>
-      <c r="S23" s="76"/>
-      <c r="T23" s="76"/>
-      <c r="U23" s="76"/>
+      <c r="Q23" s="81"/>
+      <c r="R23" s="81"/>
+      <c r="S23" s="81"/>
+      <c r="T23" s="81"/>
+      <c r="U23" s="81"/>
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
       <c r="X23" s="17"/>
@@ -4055,27 +5851,27 @@
         <v>440</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="E24" s="86" t="s">
+      <c r="E24" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="88"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="80"/>
       <c r="O24" s="9"/>
-      <c r="P24" s="76" t="s">
+      <c r="P24" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q24" s="76"/>
-      <c r="R24" s="76"/>
-      <c r="S24" s="76"/>
-      <c r="T24" s="76"/>
-      <c r="U24" s="76"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
+      <c r="U24" s="81"/>
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="19"/>
@@ -4098,27 +5894,27 @@
         <v>460</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="E25" s="86" t="s">
+      <c r="E25" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="88"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="80"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="76" t="s">
+      <c r="P25" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="76"/>
-      <c r="S25" s="76"/>
-      <c r="T25" s="76"/>
-      <c r="U25" s="76"/>
+      <c r="Q25" s="81"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
       <c r="X25" s="19"/>
@@ -4141,27 +5937,27 @@
         <v>480</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="E26" s="86" t="s">
+      <c r="E26" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="88"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="80"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="76" t="s">
+      <c r="P26" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="76"/>
-      <c r="S26" s="76"/>
-      <c r="T26" s="76"/>
-      <c r="U26" s="76"/>
+      <c r="Q26" s="81"/>
+      <c r="R26" s="81"/>
+      <c r="S26" s="81"/>
+      <c r="T26" s="81"/>
+      <c r="U26" s="81"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="19"/>
@@ -4186,27 +5982,27 @@
         <v>500</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="E27" s="86" t="s">
+      <c r="E27" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="88"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="80"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="76" t="s">
+      <c r="P27" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="76"/>
-      <c r="U27" s="76"/>
+      <c r="Q27" s="81"/>
+      <c r="R27" s="81"/>
+      <c r="S27" s="81"/>
+      <c r="T27" s="81"/>
+      <c r="U27" s="81"/>
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
       <c r="X27" s="19"/>
@@ -4229,27 +6025,27 @@
         <v>520</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="88"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="80"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="76" t="s">
+      <c r="P28" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
-      <c r="S28" s="76"/>
-      <c r="T28" s="76"/>
-      <c r="U28" s="76"/>
+      <c r="Q28" s="81"/>
+      <c r="R28" s="81"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="19"/>
@@ -4272,27 +6068,27 @@
         <v>540</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="E29" s="86" t="s">
+      <c r="E29" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="88"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="80"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="76" t="s">
+      <c r="P29" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q29" s="76"/>
-      <c r="R29" s="76"/>
-      <c r="S29" s="76"/>
-      <c r="T29" s="76"/>
-      <c r="U29" s="76"/>
+      <c r="Q29" s="81"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="25"/>
@@ -4315,23 +6111,23 @@
         <v>560</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
       <c r="O30" s="9"/>
-      <c r="P30" s="106"/>
-      <c r="Q30" s="106"/>
-      <c r="R30" s="106"/>
-      <c r="S30" s="106"/>
-      <c r="T30" s="106"/>
-      <c r="U30" s="106"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="82"/>
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
@@ -4517,6 +6313,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="P25:U25"/>
+    <mergeCell ref="P26:U26"/>
+    <mergeCell ref="P27:U27"/>
+    <mergeCell ref="P28:U28"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="P19:U19"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="P21:U21"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="X5:AD5"/>
+    <mergeCell ref="E15:U16"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="E19:N19"/>
+    <mergeCell ref="E20:N20"/>
+    <mergeCell ref="N4:U5"/>
+    <mergeCell ref="N11:R13"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="T12:U13"/>
     <mergeCell ref="E30:N30"/>
     <mergeCell ref="E17:N17"/>
     <mergeCell ref="P17:U17"/>
@@ -4533,32 +6347,14 @@
     <mergeCell ref="P30:U30"/>
     <mergeCell ref="P23:U23"/>
     <mergeCell ref="P24:U24"/>
-    <mergeCell ref="X5:AD5"/>
-    <mergeCell ref="E15:U16"/>
-    <mergeCell ref="E18:N18"/>
-    <mergeCell ref="E19:N19"/>
-    <mergeCell ref="E20:N20"/>
-    <mergeCell ref="N4:U5"/>
-    <mergeCell ref="N11:R13"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="T12:U13"/>
-    <mergeCell ref="P25:U25"/>
-    <mergeCell ref="P26:U26"/>
-    <mergeCell ref="P27:U27"/>
-    <mergeCell ref="P28:U28"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="P19:U19"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="P21:U21"/>
-    <mergeCell ref="P22:U22"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C42FEC7-1E25-498F-90C7-570E25F143D7}">
   <dimension ref="B1:AG32"/>
   <sheetViews>
@@ -6026,13 +7822,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DF39AB-3FA3-45BF-8B66-EFD455A47D2B}">
   <dimension ref="B1:AJ32"/>
   <sheetViews>
@@ -7501,14 +9297,14 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC17B423-D652-4B30-97BA-0C7E38C2D8D1}">
   <dimension ref="B1:AG32"/>
   <sheetViews>
@@ -8976,13 +10772,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C82939-DA75-4A90-AD79-9A7EEAD3011C}">
   <dimension ref="B1:AG32"/>
   <sheetViews>
@@ -9209,25 +11005,25 @@
       </c>
       <c r="C4" s="59"/>
       <c r="D4" s="38"/>
-      <c r="E4" s="107" t="s">
+      <c r="E4" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="109"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="111"/>
       <c r="K4" s="68" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="38"/>
       <c r="M4" s="38"/>
-      <c r="N4" s="110" t="s">
+      <c r="N4" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
       <c r="R4" s="68" t="s">
         <v>32</v>
       </c>
@@ -9300,28 +11096,28 @@
       <c r="E6" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="111"/>
-      <c r="V6" s="111"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
-      <c r="Y6" s="111"/>
-      <c r="Z6" s="111"/>
-      <c r="AA6" s="111"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="75"/>
       <c r="AB6" s="62"/>
       <c r="AC6" s="38"/>
       <c r="AD6" s="38"/>
@@ -10464,7 +12260,7 @@
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="N4:Q4"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>